<commit_message>
change value of C147 capacitor and change some footprint
</commit_message>
<xml_diff>
--- a/Zeabus-Elec-Hydrophone-BOM.xlsx
+++ b/Zeabus-Elec-Hydrophone-BOM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Copy\AUV\Zeabus-Elec-Hydrophone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Zeabus-Elec-Hydrophone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -563,7 +563,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -582,21 +582,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Tahoma"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -604,7 +604,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -612,7 +612,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -620,35 +620,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -656,7 +656,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -664,14 +664,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -679,14 +679,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -694,7 +694,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -702,21 +702,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1309,48 +1309,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - ส่วนที่ถูกเน้น1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="เซลล์ตรวจสอบ" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="เซลล์ที่มีลิงก์" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="แย่" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="แสดงผล" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="การคำนวณ" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="ข้อความเตือน" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="ข้อความอธิบาย" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="ชื่อเรื่อง" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="ดี" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
-    <cellStyle name="ป้อนค่า" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="ปานกลาง" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="ผลรวม" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="หมายเหตุ" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="หัวเรื่อง 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="หัวเรื่อง 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="หัวเรื่อง 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="หัวเรื่อง 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1366,7 +1366,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1667,20 +1667,20 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" style="20" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
     <col min="3" max="3" width="9" style="13"/>
-    <col min="4" max="4" width="56.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>9</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="114" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>15</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>17</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>20</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>24</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>27</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>29</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>31</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>33</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>36</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>39</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>41</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>43</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>45</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>48</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>51</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>53</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>55</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>58</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>165</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>178</v>
       </c>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>65</v>
       </c>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="E28" s="10"/>
     </row>
-    <row r="29" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>66</v>
       </c>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="E29" s="10"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>67</v>
       </c>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>68</v>
       </c>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>69</v>
       </c>
@@ -2212,7 +2212,7 @@
       </c>
       <c r="E32" s="10"/>
     </row>
-    <row r="33" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>71</v>
       </c>
@@ -2227,7 +2227,7 @@
       </c>
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>73</v>
       </c>
@@ -2242,7 +2242,7 @@
       </c>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>75</v>
       </c>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="E35" s="10"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>76</v>
       </c>
@@ -2272,7 +2272,7 @@
       </c>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>78</v>
       </c>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="E37" s="10"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>79</v>
       </c>
@@ -2302,7 +2302,7 @@
       </c>
       <c r="E38" s="10"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>80</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="E39" s="10"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>81</v>
       </c>
@@ -2332,7 +2332,7 @@
       </c>
       <c r="E40" s="10"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>83</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>84</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>87</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>90</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>93</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>96</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>99</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>102</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>105</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>108</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>111</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>114</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>116</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>119</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>122</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>124</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>127</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>130</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>133</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>136</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>139</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18" t="s">
         <v>142</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="19"/>
       <c r="B63" s="3"/>
       <c r="C63" s="12"/>

</xml_diff>